<commit_message>
outline added, part list corrected, resistor tag added, continuity check
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>NUMBER OF BOARDS</t>
   </si>
@@ -72,9 +72,6 @@
     <t>4 dip switch</t>
   </si>
   <si>
-    <t>https://www.tme.eu/cz/en/details/sda04h0sb/dip-switches/c-k/</t>
-  </si>
-  <si>
     <t>wires female</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>HEADER 8</t>
   </si>
   <si>
-    <t>advanced</t>
-  </si>
-  <si>
     <t>100kR</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>10pF</t>
   </si>
   <si>
-    <t>https://www.tme.eu/cz/en/details/pf1a471mp508b5/105degc-tht-electrolytic-capacitors/elite/pf1a471mnn08b5/</t>
-  </si>
-  <si>
     <t>ceramic cap</t>
   </si>
   <si>
@@ -160,6 +151,15 @@
   </si>
   <si>
     <t>150R</t>
+  </si>
+  <si>
+    <t>ADVANCED</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/cz/en/details/ds1052-302b2ma2015/ribbon-cables-with-idc-connectors/connfly/ds1052-302b2ma201501/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/cz/en/details/ds-04/dip-switches/ninigi/</t>
   </si>
 </sst>
 </file>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -574,7 +574,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -604,7 +604,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="3">
         <f>$D$1*C3</f>
@@ -614,7 +614,7 @@
     <row r="4" spans="1:12">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2">
         <v>4</v>
@@ -625,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -636,7 +636,7 @@
     <row r="5" spans="1:12">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -647,14 +647,15 @@
         <v>3</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> ROUNDUP($C$24/8, 0)*$D$1</f>
         <v>22</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>22</v>
+      <c r="I5" s="8" t="str">
+        <f>D25</f>
+        <v>https://www.tme.eu/cz/en/details/zl201-08g/pin-headers/connfly/ds1021-1-8sf11-b/</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -674,14 +675,15 @@
         <v>3</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H6" s="7">
         <f>E3+E6+E4+E5</f>
         <v>14</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>40</v>
+      <c r="I6" s="8" t="str">
+        <f>D3</f>
+        <v>https://www.gme.cz/ru-22k-0207-0-25w-5</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -690,27 +692,28 @@
     <row r="7" spans="1:12">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H7" s="7">
         <f>E7+E8</f>
         <v>4</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>41</v>
+      <c r="I7" s="8" t="str">
+        <f>D7</f>
+        <v>https://www.gme.cz/ck-6-8n-50v-x7r-rm5-08-10-hitano</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -719,7 +722,7 @@
     <row r="8" spans="1:12">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -730,14 +733,15 @@
         <v>2</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H8" s="7">
         <f>E9</f>
         <v>3</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>42</v>
+      <c r="I8" s="8" t="str">
+        <f>D9</f>
+        <v>https://www.gme.cz/ce-100u-25v-hit-ecr-6-3x11-rm2-5-bulk</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -746,27 +750,28 @@
     <row r="9" spans="1:12">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H9" s="7">
         <f>E11</f>
         <v>1</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>34</v>
+      <c r="I9" s="8" t="str">
+        <f>D11</f>
+        <v>https://www.tme.eu/cz/en/details/pic16f15256-i_sp/8-bit-pic-family/microchip-technology/</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -794,8 +799,9 @@
         <f>E12</f>
         <v>2</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>6</v>
+      <c r="I10" s="8" t="str">
+        <f>D12</f>
+        <v>https://www.tme.eu/cz/en/details/sn74ahc125n/buffers-transceivers-drivers/texas-instruments/</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -804,13 +810,13 @@
     <row r="11" spans="1:12">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
@@ -823,8 +829,9 @@
         <f>E13</f>
         <v>3</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>8</v>
+      <c r="I11" s="8" t="str">
+        <f>D13</f>
+        <v>https://www.tme.eu/cz/en/details/as358p-e1/tht-operational-amplifiers/diodes-incorporated/</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -852,8 +859,9 @@
         <f>E36</f>
         <v>1</v>
       </c>
-      <c r="I12" s="8" t="s">
-        <v>18</v>
+      <c r="I12" s="8" t="str">
+        <f>D36</f>
+        <v>https://www.tme.eu/cz/en/details/ds-04/dip-switches/ninigi/</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -881,8 +889,9 @@
         <f>E37</f>
         <v>1</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>25</v>
+      <c r="I13" s="8" t="str">
+        <f>D37</f>
+        <v>https://www.tme.eu/cz/details/bpt-14x/piezosireny-s-generatorem/bestar/bpt14x/</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -901,8 +910,9 @@
         <f>E39</f>
         <v>1</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>43</v>
+      <c r="I14" s="8" t="str">
+        <f>D39</f>
+        <v>https://www.gme.cz/mikrospinac-tc-0105-t</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
@@ -921,8 +931,9 @@
         <f>E10+E40</f>
         <v>5</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>15</v>
+      <c r="I15" s="8" t="str">
+        <f>D40</f>
+        <v>https://www.tme.eu/cz/en/details/fyl-5013hd1c/tht-leds-5mm/foryard/</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -941,8 +952,9 @@
         <f>E38</f>
         <v>1</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>44</v>
+      <c r="I16" s="8" t="str">
+        <f>D38</f>
+        <v>https://www.gme.cz/rm-1k-0207-0-6w-1</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
@@ -955,14 +967,15 @@
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="G17" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H17" s="7">
         <f>E41</f>
         <v>1</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>45</v>
+      <c r="I17" s="8" t="str">
+        <f>D41</f>
+        <v>https://www.gme.cz/rm-150r-0207-0-6w-1</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -974,9 +987,17 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="7">
+        <f>C42</f>
+        <v>2</v>
+      </c>
+      <c r="I18" s="7" t="str">
+        <f>D42</f>
+        <v>https://www.tme.eu/cz/en/details/ds1052-302b2ma2015/ribbon-cables-with-idc-connectors/connfly/ds1052-302b2ma201501/</v>
+      </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
@@ -1017,7 +1038,7 @@
     <row r="22" spans="1:12">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2">
@@ -1032,7 +1053,7 @@
     <row r="23" spans="1:12">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1045,7 +1066,7 @@
     <row r="24" spans="1:12">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="3">
         <f>D22+30</f>
@@ -1068,7 +1089,7 @@
         <v>21.5</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25" s="3">
         <f>C25*$D$1</f>
@@ -1120,7 +1141,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="B31" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="3">
         <f>D22/2</f>
@@ -1164,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E36" s="3">
         <f t="shared" ref="E36:E41" si="1">$D$1*C36</f>
@@ -1179,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E37" s="3">
         <f t="shared" si="1"/>
@@ -1188,13 +1209,13 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E38" s="3">
         <f t="shared" si="1"/>
@@ -1209,7 +1230,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" si="1"/>
@@ -1233,13 +1254,13 @@
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" si="1"/>
@@ -1249,6 +1270,12 @@
     <row r="42" spans="2:5">
       <c r="B42" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1262,19 +1289,19 @@
     <hyperlink ref="D13" r:id="rId3"/>
     <hyperlink ref="D3" r:id="rId4"/>
     <hyperlink ref="D40" r:id="rId5"/>
-    <hyperlink ref="D36" r:id="rId6"/>
-    <hyperlink ref="I11" r:id="rId7"/>
-    <hyperlink ref="I12" r:id="rId8"/>
-    <hyperlink ref="I5" r:id="rId9"/>
-    <hyperlink ref="I13" r:id="rId10"/>
-    <hyperlink ref="D7" r:id="rId11"/>
-    <hyperlink ref="I10" r:id="rId12"/>
-    <hyperlink ref="D37" r:id="rId13"/>
-    <hyperlink ref="D11" r:id="rId14"/>
-    <hyperlink ref="D10" r:id="rId15"/>
-    <hyperlink ref="I15" r:id="rId16"/>
-    <hyperlink ref="I17" r:id="rId17"/>
-    <hyperlink ref="I6" r:id="rId18"/>
+    <hyperlink ref="I11" r:id="rId6" display="https://www.tme.eu/cz/en/details/as358p-e1/tht-operational-amplifiers/diodes-incorporated/"/>
+    <hyperlink ref="I12" r:id="rId7" display="https://www.tme.eu/cz/en/details/sda04h0sb/dip-switches/c-k/"/>
+    <hyperlink ref="I5" r:id="rId8" display="https://www.tme.eu/cz/en/details/zl201-08g/pin-headers/connfly/ds1021-1-8sf11-b/"/>
+    <hyperlink ref="I13" r:id="rId9" display="https://www.tme.eu/cz/details/bpt-14x/piezosireny-s-generatorem/bestar/bpt14x/"/>
+    <hyperlink ref="D7" r:id="rId10"/>
+    <hyperlink ref="I10" r:id="rId11" display="https://www.tme.eu/cz/en/details/sn74ahc125n/buffers-transceivers-drivers/texas-instruments/"/>
+    <hyperlink ref="D37" r:id="rId12"/>
+    <hyperlink ref="D11" r:id="rId13"/>
+    <hyperlink ref="D10" r:id="rId14"/>
+    <hyperlink ref="I15" r:id="rId15" display="https://www.tme.eu/cz/en/details/fyl-5013hd1c/tht-leds-5mm/foryard/"/>
+    <hyperlink ref="I17" r:id="rId16" display="https://www.gme.cz/rm-150r-0207-0-6w-1"/>
+    <hyperlink ref="I6" r:id="rId17" display="https://www.gme.cz/ru-22k-0207-0-25w-5"/>
+    <hyperlink ref="D42" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>

</xml_diff>

<commit_message>
board shrunk to 10*10 , all pads now round
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1302,9 +1302,10 @@
     <hyperlink ref="I17" r:id="rId16" display="https://www.gme.cz/rm-150r-0207-0-6w-1"/>
     <hyperlink ref="I6" r:id="rId17" display="https://www.gme.cz/ru-22k-0207-0-25w-5"/>
     <hyperlink ref="D42" r:id="rId18"/>
+    <hyperlink ref="D9" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
sligh tweaks, release verison]\
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>